<commit_message>
Physics Record almost over
</commit_message>
<xml_diff>
--- a/Semester_3/Physics_Practicals/Analysis/Experiment5/attempt1.xlsx
+++ b/Semester_3/Physics_Practicals/Analysis/Experiment5/attempt1.xlsx
@@ -9,13 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8340"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9570" windowHeight="8760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="4">
   <si>
     <t>Average</t>
   </si>
@@ -34,6 +33,9 @@
   </si>
   <si>
     <t>d</t>
+  </si>
+  <si>
+    <t>Wavelength</t>
   </si>
 </sst>
 </file>
@@ -351,18 +353,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11.85546875" customWidth="1"/>
+    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -372,8 +376,20 @@
       <c r="C1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0.62</v>
       </c>
@@ -382,15 +398,33 @@
         <v>2.5000000000000577E-3</v>
       </c>
       <c r="C2">
-        <f>AVERAGE(B2:B10)</f>
-        <v>2.5111111111111059E-3</v>
+        <v>2.8999999999999998E-3</v>
       </c>
       <c r="D2">
         <f>C2/5</f>
-        <v>5.0222222222222118E-4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5.8E-4</v>
+      </c>
+      <c r="F2">
+        <f>0.62+G2</f>
+        <v>0.62280000000000002</v>
+      </c>
+      <c r="G2">
+        <v>2.8E-3</v>
+      </c>
+      <c r="H2">
+        <f>AVERAGE(G2:G10)</f>
+        <v>2.8333333333333331E-3</v>
+      </c>
+      <c r="I2">
+        <f>H2/5</f>
+        <v>5.666666666666666E-4</v>
+      </c>
+      <c r="J2">
+        <f>H3/5</f>
+        <v>2.9814239699997189E-5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0.62250000000000005</v>
       </c>
@@ -398,8 +432,23 @@
         <f>A4-A3</f>
         <v>2.3999999999999577E-3</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C3">
+        <f>_xlfn.STDEV.P(B2:B10)</f>
+        <v>1.9116278371205379E-4</v>
+      </c>
+      <c r="F3">
+        <f>F2+G3</f>
+        <v>0.62550000000000006</v>
+      </c>
+      <c r="G3">
+        <v>2.7000000000000001E-3</v>
+      </c>
+      <c r="H3">
+        <f>_xlfn.STDEV.P(G2:G10)</f>
+        <v>1.4907119849998595E-4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0.62490000000000001</v>
       </c>
@@ -407,8 +456,23 @@
         <f t="shared" ref="B4:B10" si="0">A5-A4</f>
         <v>2.9000000000000137E-3</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F4">
+        <f>F3+G4</f>
+        <v>0.62840000000000007</v>
+      </c>
+      <c r="G4">
+        <v>2.8999999999999998E-3</v>
+      </c>
+      <c r="I4">
+        <f>I2*(10^6)</f>
+        <v>566.66666666666663</v>
+      </c>
+      <c r="J4">
+        <f>J2*(10^6)</f>
+        <v>29.814239699997188</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0.62780000000000002</v>
       </c>
@@ -416,8 +480,15 @@
         <f t="shared" si="0"/>
         <v>2.5999999999999357E-3</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F5">
+        <f t="shared" ref="F5:F11" si="1">F4+G5</f>
+        <v>0.63100000000000012</v>
+      </c>
+      <c r="G5">
+        <v>2.5999999999999999E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0.63039999999999996</v>
       </c>
@@ -425,8 +496,15 @@
         <f t="shared" si="0"/>
         <v>2.6000000000000467E-3</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F6">
+        <f t="shared" si="1"/>
+        <v>0.63390000000000013</v>
+      </c>
+      <c r="G6">
+        <v>2.8999999999999998E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0.63300000000000001</v>
       </c>
@@ -434,8 +512,15 @@
         <f t="shared" si="0"/>
         <v>2.4999999999999467E-3</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F7">
+        <f t="shared" si="1"/>
+        <v>0.63670000000000015</v>
+      </c>
+      <c r="G7">
+        <v>2.8E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>0.63549999999999995</v>
       </c>
@@ -443,8 +528,15 @@
         <f t="shared" si="0"/>
         <v>2.3000000000000798E-3</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>0.63970000000000016</v>
+      </c>
+      <c r="G8">
+        <v>3.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>0.63780000000000003</v>
       </c>
@@ -452,8 +544,15 @@
         <f t="shared" si="0"/>
         <v>2.5999999999999357E-3</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>0.64280000000000015</v>
+      </c>
+      <c r="G9">
+        <v>3.0999999999999999E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>0.64039999999999997</v>
       </c>
@@ -461,10 +560,21 @@
         <f t="shared" si="0"/>
         <v>2.1999999999999797E-3</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F10">
+        <f t="shared" si="1"/>
+        <v>0.64550000000000018</v>
+      </c>
+      <c r="G10">
+        <v>2.7000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>0.64259999999999995</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="1"/>
+        <v>0.64550000000000018</v>
       </c>
     </row>
   </sheetData>

</xml_diff>